<commit_message>
Tables, UML diagram and progress report
</commit_message>
<xml_diff>
--- a/doc/Tables.xlsx
+++ b/doc/Tables.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\Gestor-de-Historias-Clinicas\Rescatable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Desktop\ClinicalHistory\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D843B34-2D9F-4148-ABD5-836D5FFAA216}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="80">
   <si>
     <t>Table address</t>
   </si>
@@ -107,9 +108,6 @@
     <t>Foreign Key</t>
   </si>
   <si>
-    <t>User</t>
-  </si>
-  <si>
     <t>Table Doctor</t>
   </si>
   <si>
@@ -182,18 +180,9 @@
     <t>Text</t>
   </si>
   <si>
-    <t>IDillness</t>
-  </si>
-  <si>
-    <t>Idsurgery</t>
-  </si>
-  <si>
     <t>Table Surgeries</t>
   </si>
   <si>
-    <t>DOS</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -206,19 +195,76 @@
     <t>IdPatient</t>
   </si>
   <si>
-    <t>Table Ilnesses</t>
-  </si>
-  <si>
-    <t>Personal Pathologies</t>
-  </si>
-  <si>
-    <t>Hereditary disease</t>
-  </si>
-  <si>
     <t>Idpatient</t>
   </si>
   <si>
     <t>N-N relationship</t>
+  </si>
+  <si>
+    <t>Landline</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>varchar (20)</t>
+  </si>
+  <si>
+    <t>Photo</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>Columna1</t>
+  </si>
+  <si>
+    <t>Table Illnesses</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Test Results</t>
+  </si>
+  <si>
+    <t>varchar (50)</t>
+  </si>
+  <si>
+    <t>Clinical History</t>
+  </si>
+  <si>
+    <t>Addictions</t>
+  </si>
+  <si>
+    <t>Last modification</t>
+  </si>
+  <si>
+    <t>Blood group</t>
+  </si>
+  <si>
+    <t>varchar (5)</t>
+  </si>
+  <si>
+    <t>Not null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username </t>
+  </si>
+  <si>
+    <t>Usertype</t>
   </si>
 </sst>
 </file>
@@ -234,12 +280,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -254,11 +306,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -277,8 +333,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="C5:G12" totalsRowShown="0">
-  <autoFilter ref="C5:G12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="C5:G10" totalsRowShown="0">
+  <autoFilter ref="C5:G10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Data Type"/>
@@ -290,9 +346,36 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{B73098A0-6269-4343-9D2B-7439270ADB8D}" name="Tabla611" displayName="Tabla611" ref="C50:G56" totalsRowShown="0">
+  <autoFilter ref="C50:G56" xr:uid="{27906509-B6D7-4151-A252-3C9082DF7704}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A5EE567F-A693-41B7-987B-31D9E55CC005}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{BAE9A99A-0AF2-4903-9B36-4FF5024F2E74}" name="DataType"/>
+    <tableColumn id="3" xr3:uid="{93359A6F-F03D-4AE9-9280-7418AA5E84DE}" name="Primary Key"/>
+    <tableColumn id="4" xr3:uid="{BF30FD44-76D8-4F44-8625-A0A6A16A3530}" name="NotNull"/>
+    <tableColumn id="5" xr3:uid="{8A6FD308-EEDF-4DF9-9015-3E80D8B41115}" name="Foreign Key"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{3F625792-37CB-41E8-9AAA-4342A263E848}" name="Tabla12" displayName="Tabla12" ref="C60:F65" totalsRowShown="0">
+  <autoFilter ref="C60:F65" xr:uid="{AC1E83D0-444B-4784-A310-988F014F899A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3D14FC9F-5BD6-4435-BB02-BBE5108A04F0}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{2CF554BE-8ABD-4510-9257-F222D2BD2849}" name="Data Type"/>
+    <tableColumn id="3" xr3:uid="{958DC484-31B0-4566-93AC-83896E2C348E}" name="Primary Key"/>
+    <tableColumn id="4" xr3:uid="{138B4FD3-427C-4732-8F37-D95D63B9ADD3}" name="Not null"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla2" displayName="Tabla2" ref="J5:N9" totalsRowShown="0">
-  <autoFilter ref="J5:N9" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla2" displayName="Tabla2" ref="J5:N12" totalsRowShown="0">
+  <autoFilter ref="J5:N12" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Data Type"/>
@@ -305,8 +388,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla3" displayName="Tabla3" ref="C17:G29" totalsRowShown="0">
-  <autoFilter ref="C17:G29" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabla3" displayName="Tabla3" ref="C15:G29" totalsRowShown="0">
+  <autoFilter ref="C15:G29" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Data Type"/>
@@ -319,8 +402,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabla4" displayName="Tabla4" ref="J12:N21" totalsRowShown="0">
-  <autoFilter ref="J12:N21" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabla4" displayName="Tabla4" ref="J14:N27" totalsRowShown="0">
+  <autoFilter ref="J14:N27" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="DataType"/>
@@ -333,8 +416,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabla5" displayName="Tabla5" ref="J24:N33" totalsRowShown="0">
-  <autoFilter ref="J24:N33" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tabla5" displayName="Tabla5" ref="J30:N38" totalsRowShown="0">
+  <autoFilter ref="J30:N38" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="DataType"/>
@@ -361,8 +444,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabla7" displayName="Tabla7" ref="J36:N39" totalsRowShown="0">
-  <autoFilter ref="J36:N39" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tabla7" displayName="Tabla7" ref="J41:N46" totalsRowShown="0">
+  <autoFilter ref="J41:N46" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="DataType"/>
@@ -375,8 +458,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35ACFDBE-D7C0-4199-877A-AB70D0666A07}" name="Tabla79" displayName="Tabla79" ref="J43:N48" totalsRowShown="0">
-  <autoFilter ref="J43:N48" xr:uid="{8C056C3B-567E-4B6C-AF0F-942663AF5B14}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{35ACFDBE-D7C0-4199-877A-AB70D0666A07}" name="Tabla79" displayName="Tabla79" ref="J50:N57" totalsRowShown="0">
+  <autoFilter ref="J50:N57" xr:uid="{8C056C3B-567E-4B6C-AF0F-942663AF5B14}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0CC9D668-F7C2-4822-975D-A08CD15E4424}" name="Name"/>
     <tableColumn id="2" xr3:uid="{691E2027-CA78-44ED-9EB2-625BE5471C3C}" name="DataType"/>
@@ -389,14 +472,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1BD31A8E-9449-469D-BCF1-B19CC8625CEA}" name="Tabla612" displayName="Tabla612" ref="C43:G45" totalsRowShown="0">
-  <autoFilter ref="C43:G45" xr:uid="{B488CB91-00D9-43A9-AA8E-8EB014DF292A}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{1BD31A8E-9449-469D-BCF1-B19CC8625CEA}" name="Tabla612" displayName="Tabla612" ref="C43:F45" totalsRowShown="0">
+  <autoFilter ref="C43:F45" xr:uid="{B488CB91-00D9-43A9-AA8E-8EB014DF292A}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9725343F-7513-4D46-B4C3-CDBD77E58E44}" name="Name"/>
     <tableColumn id="2" xr3:uid="{FFD62CA7-CDFC-49B1-94AA-D2B5D96D2D67}" name="DataType"/>
-    <tableColumn id="3" xr3:uid="{36C4EB9E-A74F-4C2B-844C-18D1327822A8}" name="Primary Key"/>
     <tableColumn id="4" xr3:uid="{A1AA9A23-FC18-4517-87CB-36DA00740CB1}" name="NotNull"/>
-    <tableColumn id="5" xr3:uid="{5E9ABA0D-C5BD-4288-918D-E9F4B981464A}" name="Foreign Key"/>
+    <tableColumn id="5" xr3:uid="{5E9ABA0D-C5BD-4288-918D-E9F4B981464A}" name="Columna1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -699,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:N48"/>
+  <dimension ref="C4:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -720,20 +802,20 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
@@ -848,106 +930,100 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M12" t="s">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="J13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="N12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="J13" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" t="s">
-        <v>13</v>
-      </c>
-      <c r="M13" t="s">
-        <v>13</v>
-      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
       <c r="J14" t="s">
         <v>1</v>
       </c>
       <c r="K14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" t="s">
+        <v>38</v>
+      </c>
+      <c r="N14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
         <v>4</v>
       </c>
-      <c r="M14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="J15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
         <v>4</v>
-      </c>
-      <c r="M15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" t="s">
-        <v>20</v>
       </c>
       <c r="M16" t="s">
         <v>13</v>
@@ -955,30 +1031,30 @@
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="J17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="K17" t="s">
-        <v>36</v>
+        <v>4</v>
+      </c>
+      <c r="M17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -987,258 +1063,227 @@
         <v>13</v>
       </c>
       <c r="J18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="M18" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C19" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="K19" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C20" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="K20" t="s">
-        <v>10</v>
-      </c>
-      <c r="M20" t="s">
-        <v>13</v>
-      </c>
-      <c r="N20" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="K21" t="s">
-        <v>10</v>
-      </c>
-      <c r="M21" t="s">
-        <v>13</v>
-      </c>
-      <c r="N21" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>4</v>
+      </c>
+      <c r="J22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" t="s">
+        <v>10</v>
+      </c>
+      <c r="M22" t="s">
+        <v>13</v>
+      </c>
+      <c r="N22" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
       </c>
       <c r="J24" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="K24" t="s">
-        <v>35</v>
-      </c>
-      <c r="L24" t="s">
-        <v>11</v>
-      </c>
-      <c r="M24" t="s">
-        <v>39</v>
-      </c>
-      <c r="N24" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
       <c r="J25" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="K25" t="s">
-        <v>10</v>
-      </c>
-      <c r="L25" t="s">
-        <v>13</v>
-      </c>
-      <c r="M25" t="s">
-        <v>13</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="J26" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="K26" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
         <v>10</v>
       </c>
-      <c r="F27" t="s">
-        <v>13</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" t="s">
-        <v>46</v>
-      </c>
-      <c r="K27" t="s">
-        <v>41</v>
-      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
-      </c>
-      <c r="J28" t="s">
-        <v>47</v>
-      </c>
-      <c r="K28" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>13</v>
-      </c>
-      <c r="J29" t="s">
-        <v>48</v>
-      </c>
-      <c r="K29" t="s">
-        <v>51</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.45">
       <c r="J30" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="K30" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="L30" t="s">
+        <v>11</v>
+      </c>
+      <c r="M30" t="s">
+        <v>38</v>
+      </c>
+      <c r="N30" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.45">
       <c r="J31" t="s">
-        <v>52</v>
+        <v>9</v>
       </c>
       <c r="K31" t="s">
         <v>10</v>
       </c>
+      <c r="L31" t="s">
+        <v>13</v>
+      </c>
       <c r="M31" t="s">
         <v>13</v>
       </c>
-      <c r="N31" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="C32" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="C32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
       <c r="J32" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="K32" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="M32" t="s">
-        <v>13</v>
-      </c>
-      <c r="N32" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1247,24 +1292,24 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" t="s">
         <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="K33" t="s">
-        <v>10</v>
-      </c>
-      <c r="N33" t="s">
+        <v>40</v>
+      </c>
+      <c r="M33" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1281,43 +1326,39 @@
       <c r="F34" t="s">
         <v>13</v>
       </c>
+      <c r="J34" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
-      </c>
-      <c r="J35" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="J35" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
       </c>
       <c r="J36" t="s">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="K36" t="s">
-        <v>35</v>
-      </c>
-      <c r="L36" t="s">
-        <v>11</v>
-      </c>
-      <c r="M36" t="s">
-        <v>39</v>
-      </c>
-      <c r="N36" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.45">
@@ -1334,92 +1375,97 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="K37" t="s">
         <v>10</v>
       </c>
-      <c r="L37" t="s">
+      <c r="M37" t="s">
+        <v>13</v>
+      </c>
+      <c r="N37" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" t="s">
+        <v>70</v>
+      </c>
+      <c r="K38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="J40" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="J41" t="s">
+        <v>1</v>
+      </c>
+      <c r="K41" t="s">
+        <v>34</v>
+      </c>
+      <c r="L41" t="s">
+        <v>11</v>
+      </c>
+      <c r="M41" t="s">
+        <v>38</v>
+      </c>
+      <c r="N41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="D42" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="F38" t="s">
-        <v>13</v>
-      </c>
-      <c r="G38" t="s">
-        <v>13</v>
-      </c>
-      <c r="J38" t="s">
-        <v>1</v>
-      </c>
-      <c r="K38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="J39" t="s">
-        <v>59</v>
-      </c>
-      <c r="K39" t="s">
-        <v>10</v>
-      </c>
-      <c r="M39" t="s">
-        <v>13</v>
-      </c>
-      <c r="N39" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="D42" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="J42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="E42" s="2"/>
+      <c r="J42" t="s">
+        <v>9</v>
+      </c>
+      <c r="K42" t="s">
+        <v>10</v>
+      </c>
+      <c r="L42" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="43" spans="3:14" x14ac:dyDescent="0.45">
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="F43" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="J43" t="s">
         <v>1</v>
       </c>
       <c r="K43" t="s">
-        <v>35</v>
-      </c>
-      <c r="L43" t="s">
-        <v>11</v>
-      </c>
-      <c r="M43" t="s">
-        <v>39</v>
-      </c>
-      <c r="N43" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="3:14" x14ac:dyDescent="0.45">
@@ -1432,19 +1478,17 @@
       <c r="E44" t="s">
         <v>13</v>
       </c>
-      <c r="F44" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" t="s">
-        <v>13</v>
-      </c>
+      <c r="I44" s="1"/>
       <c r="J44" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="K44" t="s">
         <v>10</v>
       </c>
-      <c r="L44" t="s">
+      <c r="M44" t="s">
+        <v>13</v>
+      </c>
+      <c r="N44" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1458,66 +1502,258 @@
       <c r="E45" t="s">
         <v>13</v>
       </c>
-      <c r="F45" t="s">
-        <v>13</v>
-      </c>
-      <c r="G45" t="s">
-        <v>13</v>
-      </c>
       <c r="J45" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="K45" t="s">
-        <v>10</v>
-      </c>
-      <c r="M45" t="s">
-        <v>13</v>
-      </c>
-      <c r="N45" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="3:14" x14ac:dyDescent="0.45">
       <c r="J46" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="K46" t="s">
-        <v>51</v>
-      </c>
-      <c r="M46" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="J47" t="s">
-        <v>61</v>
-      </c>
-      <c r="K47" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="48" spans="3:14" x14ac:dyDescent="0.45">
-      <c r="J48" t="s">
-        <v>62</v>
-      </c>
-      <c r="K48" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>34</v>
+      </c>
+      <c r="E50" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" t="s">
+        <v>38</v>
+      </c>
+      <c r="G50" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" t="s">
+        <v>1</v>
+      </c>
+      <c r="K50" t="s">
+        <v>34</v>
+      </c>
+      <c r="L50" t="s">
+        <v>11</v>
+      </c>
+      <c r="M50" t="s">
+        <v>38</v>
+      </c>
+      <c r="N50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="s">
+        <v>13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C52" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>9</v>
+      </c>
+      <c r="K52" t="s">
+        <v>10</v>
+      </c>
+      <c r="L52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>55</v>
+      </c>
+      <c r="K53" t="s">
+        <v>10</v>
+      </c>
+      <c r="M53" t="s">
+        <v>13</v>
+      </c>
+      <c r="N53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+      <c r="J54" t="s">
+        <v>48</v>
+      </c>
+      <c r="K54" t="s">
+        <v>50</v>
+      </c>
+      <c r="M54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C55" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C56" t="s">
+        <v>75</v>
+      </c>
+      <c r="D56" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" t="s">
+        <v>13</v>
+      </c>
+      <c r="J56" t="s">
+        <v>40</v>
+      </c>
+      <c r="K56" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="57" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="J57" t="s">
+        <v>53</v>
+      </c>
+      <c r="K57" t="s">
+        <v>10</v>
+      </c>
+      <c r="N57" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
+        <v>2</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C63" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="3:14" x14ac:dyDescent="0.45">
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.45">
+      <c r="C65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="J42:N42"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C49:G49"/>
     <mergeCell ref="D42:E42"/>
-    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="J29:N29"/>
     <mergeCell ref="C32:G32"/>
-    <mergeCell ref="J35:N35"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="J40:N40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="9">
+  <tableParts count="11">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -1527,6 +1763,8 @@
     <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>